<commit_message>
:bug: bugfix: excel & get-by-date
</commit_message>
<xml_diff>
--- a/forms-coleta/src/main/java/com/wise/forms_coleta/implementations/excel/excel_file/coletas.xlsx
+++ b/forms-coleta/src/main/java/com/wise/forms_coleta/implementations/excel/excel_file/coletas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Técnico</t>
   </si>
@@ -36,6 +36,12 @@
     <t>PT-01</t>
   </si>
   <si>
+    <t>PB-02</t>
+  </si>
+  <si>
+    <t>PB-03</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -81,10 +87,16 @@
     <t>08:00</t>
   </si>
   <si>
-    <t>16:46:32.168</t>
+    <t>09:47:59.460</t>
   </si>
   <si>
     <t>ETAS</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:32:42.884</t>
   </si>
   <si>
     <t>Sensor de pH PHIT-SE.01.1</t>
@@ -359,7 +371,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -368,6 +380,8 @@
     <col min="5" max="5" width="16.9296875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="25.30078125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="6.8203125" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" width="25.30078125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="25.30078125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="15.8359375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.6875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="16.15625" customWidth="true" bestFit="true"/>
@@ -376,6 +390,14 @@
     <col min="12" max="12" width="34.99609375" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="7.0078125" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="21.0703125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="16.15625" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" width="16.60546875" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="15.58203125" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="34.99609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.15625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.60546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="15.58203125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="34.99609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -400,66 +422,102 @@
       <c r="M1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="P1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="U1" t="s" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="P2" t="s" s="3">
         <v>13</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="Q2" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="R2" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="S2" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="N2" t="s" s="3">
+      <c r="T2" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="O2" t="s" s="3">
-        <v>18</v>
+      <c r="U2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="W2" t="s" s="3">
+        <v>15</v>
+      </c>
+      <c r="X2" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s" s="3">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" t="n" s="1">
         <v>1.0</v>
@@ -468,7 +526,7 @@
         <v>2.0</v>
       </c>
       <c r="G3" t="s" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n" s="1">
         <v>10.0</v>
@@ -494,12 +552,58 @@
       <c r="O3" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="P3" t="n" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="Q3" t="n" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="R3" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="S3" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="T3" t="n" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="1">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="1">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="1">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E4" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F4" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G4" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="H4" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="I4" t="n" s="1">
+        <v>10.0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -573,197 +677,197 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U1" t="s" s="2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="V1" t="s" s="2">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AB1" t="s" s="2">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AE1" t="s" s="2">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AO1" t="s" s="2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AQ1" t="s" s="2">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AR1" t="s" s="2">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s" s="3">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s" s="3">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s" s="3">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s" s="3">
+        <v>50</v>
+      </c>
+      <c r="O2" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s" s="3">
         <v>45</v>
       </c>
-      <c r="N2" t="s" s="3">
-        <v>46</v>
-      </c>
-      <c r="O2" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="P2" t="s" s="3">
-        <v>41</v>
-      </c>
       <c r="Q2" t="s" s="3">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s" s="3">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="S2" t="s" s="3">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="T2" t="s" s="3">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="U2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="V2" t="s" s="3">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="W2" t="s" s="3">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="X2" t="s" s="3">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Y2" t="s" s="3">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s" s="3">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AA2" t="s" s="3">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AB2" t="s" s="3">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AC2" t="s" s="3">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AD2" t="s" s="3">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AE2" t="s" s="3">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AF2" t="s" s="3">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AG2" t="s" s="3">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AH2" t="s" s="3">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AI2" t="s" s="3">
+        <v>68</v>
+      </c>
+      <c r="AJ2" t="s" s="3">
         <v>64</v>
       </c>
-      <c r="AJ2" t="s" s="3">
-        <v>60</v>
-      </c>
       <c r="AK2" t="s" s="3">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AL2" t="s" s="3">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AM2" t="s" s="3">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AN2" t="s" s="3">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AO2" t="s" s="3">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AP2" t="s" s="3">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AQ2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AR2" t="s" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" t="n" s="1">
         <v>70.0</v>
@@ -772,10 +876,10 @@
         <v>30.0</v>
       </c>
       <c r="G3" t="s" s="1">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s" s="1">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I3" t="n" s="1">
         <v>10.0</v>
@@ -796,7 +900,7 @@
         <v>10.0</v>
       </c>
       <c r="O3" t="s" s="1">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P3" t="n" s="1">
         <v>40.0</v>
@@ -814,7 +918,7 @@
         <v>20.0</v>
       </c>
       <c r="U3" t="s" s="1">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="V3" t="n" s="1">
         <v>10.0</v>
@@ -829,10 +933,10 @@
         <v>40.0</v>
       </c>
       <c r="Z3" t="s" s="1">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AA3" t="s" s="1">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AB3" t="n" s="1">
         <v>5.0</v>
@@ -844,7 +948,7 @@
         <v>15.0</v>
       </c>
       <c r="AE3" t="s" s="1">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AF3" t="n" s="1">
         <v>1.0</v>
@@ -859,7 +963,7 @@
         <v>30.0</v>
       </c>
       <c r="AJ3" t="s" s="1">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AK3" t="n" s="1">
         <v>1.0</v>
@@ -874,10 +978,10 @@
         <v>4.0</v>
       </c>
       <c r="AO3" t="s" s="1">
+        <v>78</v>
+      </c>
+      <c r="AP3" t="s" s="1">
         <v>74</v>
-      </c>
-      <c r="AP3" t="s" s="1">
-        <v>70</v>
       </c>
       <c r="AQ3" t="n" s="1">
         <v>5.0</v>

</xml_diff>

<commit_message>
:bug: bugfix: exportar excel (pm / pt)
</commit_message>
<xml_diff>
--- a/forms-coleta/src/main/java/com/wise/forms_coleta/implementations/excel/excel_file/coletas.xlsx
+++ b/forms-coleta/src/main/java/com/wise/forms_coleta/implementations/excel/excel_file/coletas.xlsx
@@ -1,16 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
-  <sheets/>
+  <sheets>
+    <sheet name="DADOS ETAS" r:id="rId3" sheetId="1"/>
+  </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+  <si>
+    <t>Técnico</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hora Início</t>
+  </si>
+  <si>
+    <t>Hora Fim</t>
+  </si>
+  <si>
+    <t>PB-01</t>
+  </si>
+  <si>
+    <t>PM-01</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pressão PI-B.01.1 (kgf/cm²)</t>
+  </si>
+  <si>
+    <t>Pulsos PQ-B.01.1</t>
+  </si>
+  <si>
+    <t>Nível de Óleo (m)</t>
+  </si>
+  <si>
+    <t>Nível d'água (m)</t>
+  </si>
+  <si>
+    <t>Volume Manual Removido de Óleo (L)</t>
+  </si>
+  <si>
+    <t>NA(m)</t>
+  </si>
+  <si>
+    <t>NO(m)</t>
+  </si>
+  <si>
+    <t>FL REMO. MANUAL (L)</t>
+  </si>
+  <si>
+    <t>BOSCH</t>
+  </si>
+  <si>
+    <t>2024-09-05</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>13:21:53.215</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -126,4 +186,131 @@
     </xf>
   </cellXfs>
 </styleSheet>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="true"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="5" max="5" width="25.30078125" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="6.8203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="16.15625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.60546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="15.58203125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="34.99609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="7.0078125" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="21.0703125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="1">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>18</v>
+      </c>
+      <c r="E3" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F3" t="n" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="G3" t="n" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="H3" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I3" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J3" t="n" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="K3" t="n" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L3" t="n" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>